<commit_message>
Refactored import excel file
</commit_message>
<xml_diff>
--- a/db_tools/acctg_db2/acctg_export2.xlsx
+++ b/db_tools/acctg_db2/acctg_export2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\acctg_db2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349C920D-BEAD-4864-8773-9E7498784BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7B909A-E56B-455E-85F6-879F7AB4389A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="account_types" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,28 @@
     <sheet name="bill_payments" sheetId="19" r:id="rId20"/>
     <sheet name="bank_transactions" sheetId="20" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <externalReferences>
+    <externalReference r:id="rId22"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="681">
   <si>
     <t>id</t>
   </si>
@@ -2114,7 +2130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2137,6 +2153,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2146,8 +2173,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2163,6 +2192,513 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Accounts"/>
+      <sheetName val="Customers"/>
+      <sheetName val="Invoice_Payments"/>
+      <sheetName val="Invoices"/>
+      <sheetName val="Received_Moneys"/>
+      <sheetName val="Invoice_Lines"/>
+      <sheetName val="Received_Money_Lines"/>
+      <sheetName val="Suppliers"/>
+      <sheetName val="Bill_Payments"/>
+      <sheetName val="Bills"/>
+      <sheetName val="Bill_Lines"/>
+      <sheetName val="Spent_Moneys"/>
+      <sheetName val="Spent_Money_Lines"/>
+      <sheetName val="Journals"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>110</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>Business Bank Account</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>120</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Accounts Receivable</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>130</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Petty Cash</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>135</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>Provision for Doubtful Debts</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>140</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>Prepayments</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>150</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>Withholding Tax Paid</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>160</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>Inventory</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>165</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>Provision for Stock Obsolence</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>170</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>Land</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>180</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>Building</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>185</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Accumulated Depreciation on Building</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>190</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>Office Equipment</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>195</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>Accumulated Depreciation on Office Equipment</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>200</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>Computer Equipment</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>205</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>Accumulated Depreciation on Computer Equipment</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>210</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>Furniture</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>215</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>Accumulated Depreciation on Furniture</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>220</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>Motor Vehicles</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>225</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>Accumulated Depreciation on Motor Vehicles</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>310</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>Accounts Payable</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>320</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>Accrued Expenses</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>330</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>Revenue Received in Advance</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>340</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>Wages Payable - Payroll</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>350</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>Wages Deductions Payable</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>360</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>Income Tax</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>370</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>Finance Lease</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>380</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>Loans Payable</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>410</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>Owner - Investments</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>420</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>Owner - Drawings</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>430</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>Retained Earnings</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>510</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>Sales</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>520</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>Other Revenue</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>530</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>Interest Income</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>540</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>Dividends Received</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>610</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>Cost of Goods Sold</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>620</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>General Expenses</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>630</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>Supplies Expense</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>640</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>Advertising</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>650</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>Consulting &amp; Accounting</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>660</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>Depreciation</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>670</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>Entertainment</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>680</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>Freight &amp; Courier</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>690</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>Insurance</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>700</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>Legal expenses</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>710</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>Electricity</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>720</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>Motor Vehicle Expenses</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>730</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>Office Expenses</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>740</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>Printing &amp; Stationery</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>750</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>Rates</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>760</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>Rent</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>770</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>Repairs and Maintenance</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>780</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>Salaries</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>790</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>Subscriptions</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>800</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>Telephone &amp; Internet</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>810</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>Travel Expenses</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>820</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>Bank Fees</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>830</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>Interest Expense</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>840</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>Income Tax Expense</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4346,7 +4882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5787,10 +6323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5805,7 +6341,7 @@
     <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5830,8 +6366,11 @@
       <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5853,8 +6392,12 @@
       <c r="H2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="str">
+        <f>_xlfn.XLOOKUP(C2,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5879,8 +6422,12 @@
       <c r="H3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="str">
+        <f>_xlfn.XLOOKUP(C3,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5905,8 +6452,12 @@
       <c r="H4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="str">
+        <f>_xlfn.XLOOKUP(C4,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5931,8 +6482,12 @@
       <c r="H5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="str">
+        <f>_xlfn.XLOOKUP(C5,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5957,8 +6512,12 @@
       <c r="H6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="str">
+        <f>_xlfn.XLOOKUP(C6,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5983,8 +6542,12 @@
       <c r="H7" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="str">
+        <f>_xlfn.XLOOKUP(C7,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6009,8 +6572,12 @@
       <c r="H8" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <f>_xlfn.XLOOKUP(C8,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6035,8 +6602,12 @@
       <c r="H9" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <f>_xlfn.XLOOKUP(C9,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6061,8 +6632,12 @@
       <c r="H10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="str">
+        <f>_xlfn.XLOOKUP(C10,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6087,8 +6662,12 @@
       <c r="H11" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="str">
+        <f>_xlfn.XLOOKUP(C11,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6113,8 +6692,12 @@
       <c r="H12" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="str">
+        <f>_xlfn.XLOOKUP(C12,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6139,8 +6722,12 @@
       <c r="H13" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="str">
+        <f>_xlfn.XLOOKUP(C13,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6165,8 +6752,12 @@
       <c r="H14" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="str">
+        <f>_xlfn.XLOOKUP(C14,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6191,8 +6782,12 @@
       <c r="H15" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="str">
+        <f>_xlfn.XLOOKUP(C15,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6217,8 +6812,12 @@
       <c r="H16" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <f>_xlfn.XLOOKUP(C16,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6243,8 +6842,12 @@
       <c r="H17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="str">
+        <f>_xlfn.XLOOKUP(C17,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6266,8 +6869,12 @@
       <c r="H18" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="str">
+        <f>_xlfn.XLOOKUP(C18,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6292,8 +6899,12 @@
       <c r="H19" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" t="str">
+        <f>_xlfn.XLOOKUP(C19,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6318,8 +6929,12 @@
       <c r="H20" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <f>_xlfn.XLOOKUP(C20,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6344,8 +6959,12 @@
       <c r="H21" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <f>_xlfn.XLOOKUP(C21,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6370,8 +6989,12 @@
       <c r="H22" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" t="str">
+        <f>_xlfn.XLOOKUP(C22,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6396,8 +7019,12 @@
       <c r="H23" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" t="str">
+        <f>_xlfn.XLOOKUP(C23,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6422,8 +7049,12 @@
       <c r="H24" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" t="str">
+        <f>_xlfn.XLOOKUP(C24,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6448,8 +7079,12 @@
       <c r="H25" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" t="str">
+        <f>_xlfn.XLOOKUP(C25,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6474,8 +7109,12 @@
       <c r="H26" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" t="str">
+        <f>_xlfn.XLOOKUP(C26,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6500,8 +7139,12 @@
       <c r="H27" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" t="str">
+        <f>_xlfn.XLOOKUP(C27,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6523,8 +7166,12 @@
       <c r="H28" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" t="str">
+        <f>_xlfn.XLOOKUP(C28,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6549,8 +7196,12 @@
       <c r="H29" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" t="str">
+        <f>_xlfn.XLOOKUP(C29,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6575,8 +7226,12 @@
       <c r="H30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <f>_xlfn.XLOOKUP(C30,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6601,8 +7256,12 @@
       <c r="H31" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" t="str">
+        <f>_xlfn.XLOOKUP(C31,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6624,8 +7283,12 @@
       <c r="H32" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" t="str">
+        <f>_xlfn.XLOOKUP(C32,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6650,8 +7313,12 @@
       <c r="H33" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="str">
+        <f>_xlfn.XLOOKUP(C33,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6676,8 +7343,12 @@
       <c r="H34" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" t="str">
+        <f>_xlfn.XLOOKUP(C34,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6702,8 +7373,12 @@
       <c r="H35" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35">
+        <f>_xlfn.XLOOKUP(C35,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6728,8 +7403,12 @@
       <c r="H36" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" t="str">
+        <f>_xlfn.XLOOKUP(C36,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6751,8 +7430,12 @@
       <c r="H37" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" t="str">
+        <f>_xlfn.XLOOKUP(C37,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6777,8 +7460,12 @@
       <c r="H38" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <f>_xlfn.XLOOKUP(C38,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6803,8 +7490,12 @@
       <c r="H39" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" t="str">
+        <f>_xlfn.XLOOKUP(C39,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6829,8 +7520,12 @@
       <c r="H40" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" t="str">
+        <f>_xlfn.XLOOKUP(C40,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6855,8 +7550,12 @@
       <c r="H41" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" t="str">
+        <f>_xlfn.XLOOKUP(C41,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6881,8 +7580,12 @@
       <c r="H42" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" t="str">
+        <f>_xlfn.XLOOKUP(C42,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6907,8 +7610,12 @@
       <c r="H43" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" t="str">
+        <f>_xlfn.XLOOKUP(C43,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6933,8 +7640,12 @@
       <c r="H44" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" t="str">
+        <f>_xlfn.XLOOKUP(C44,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6959,8 +7670,12 @@
       <c r="H45" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" t="str">
+        <f>_xlfn.XLOOKUP(C45,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6985,8 +7700,12 @@
       <c r="H46" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46">
+        <f>_xlfn.XLOOKUP(C46,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7010,6 +7729,10 @@
       </c>
       <c r="H47" t="s">
         <v>151</v>
+      </c>
+      <c r="I47" t="str">
+        <f>_xlfn.XLOOKUP(C47,[1]Accounts!$B$2:$B$59,[1]Accounts!$A$2:$A$59,"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -7021,7 +7744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -8391,7 +9116,7 @@
       <c r="M12" t="s">
         <v>637</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" t="s">
         <v>636</v>
       </c>
       <c r="O12" t="s">
@@ -8444,7 +9169,7 @@
       <c r="M13" t="s">
         <v>638</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" t="s">
         <v>636</v>
       </c>
       <c r="O13" t="s">
@@ -8497,7 +9222,7 @@
       <c r="M14" t="s">
         <v>639</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" t="s">
         <v>636</v>
       </c>
       <c r="O14" t="s">
@@ -8550,7 +9275,7 @@
       <c r="M15" t="s">
         <v>640</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="N15" t="s">
         <v>636</v>
       </c>
       <c r="O15" t="s">
@@ -8603,7 +9328,7 @@
       <c r="M16" t="s">
         <v>641</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N16" t="s">
         <v>636</v>
       </c>
       <c r="O16" t="s">
@@ -8708,7 +9433,7 @@
       <c r="D1" t="s">
         <v>644</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>645</v>
       </c>
       <c r="F1" t="s">
@@ -8766,7 +9491,7 @@
       <c r="D3" t="s">
         <v>656</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>209268717220</v>
       </c>
       <c r="F3" t="s">
@@ -8795,7 +9520,7 @@
       <c r="D4" t="s">
         <v>661</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>207555183118</v>
       </c>
       <c r="F4" t="s">
@@ -8824,7 +9549,7 @@
       <c r="D5" t="s">
         <v>666</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>208714677697</v>
       </c>
       <c r="F5" t="s">
@@ -8853,7 +9578,7 @@
       <c r="D6" t="s">
         <v>672</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>201564537686</v>
       </c>
       <c r="F6" t="s">

</xml_diff>

<commit_message>
Added final design of the database
</commit_message>
<xml_diff>
--- a/db_tools/acctg_db2/acctg_export2.xlsx
+++ b/db_tools/acctg_db2/acctg_export2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\acctg_db2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC28EBC-7403-48C7-A42A-D4D7CF0BD5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8298E5B5-7415-411C-9BED-459503CFDC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="account_types" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,9 @@
     <sheet name="journals" sheetId="10" r:id="rId11"/>
     <sheet name="journal_lines" sheetId="11" r:id="rId12"/>
     <sheet name="invoices" sheetId="14" r:id="rId13"/>
-    <sheet name="product_categories" sheetId="12" r:id="rId14"/>
-    <sheet name="products" sheetId="13" r:id="rId15"/>
-    <sheet name="invoice_lines" sheetId="15" r:id="rId16"/>
+    <sheet name="invoice_lines" sheetId="15" r:id="rId14"/>
+    <sheet name="product_categories" sheetId="12" r:id="rId15"/>
+    <sheet name="products" sheetId="13" r:id="rId16"/>
     <sheet name="bills" sheetId="16" r:id="rId17"/>
     <sheet name="bill_lines" sheetId="17" r:id="rId18"/>
     <sheet name="cash_transactions" sheetId="19" r:id="rId19"/>
@@ -2886,6 +2886,319 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1200</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>180</v>
+      </c>
+      <c r="I2">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>24.99</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>7.5</v>
+      </c>
+      <c r="I3">
+        <v>107.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>250</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>187.5</v>
+      </c>
+      <c r="I4">
+        <v>2687.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>350</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>131.25</v>
+      </c>
+      <c r="I5">
+        <v>1881.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>299.99</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>67.5</v>
+      </c>
+      <c r="I6">
+        <v>967.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>406</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>5.99</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>8.99</v>
+      </c>
+      <c r="I7">
+        <v>128.79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>409</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>225</v>
+      </c>
+      <c r="I8">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>950</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>356.25</v>
+      </c>
+      <c r="I9">
+        <v>5106.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>407</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>24.99</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="I10">
+        <v>268.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2971,7 +3284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -3527,319 +3840,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1200</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>180</v>
-      </c>
-      <c r="I2">
-        <v>2580</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>24.99</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>7.5</v>
-      </c>
-      <c r="I3">
-        <v>107.46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>404</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>250</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>187.5</v>
-      </c>
-      <c r="I4">
-        <v>2687.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>405</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>350</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>131.25</v>
-      </c>
-      <c r="I5">
-        <v>1881.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>408</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>299.99</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>67.5</v>
-      </c>
-      <c r="I6">
-        <v>967.47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>406</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>5.99</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>8.99</v>
-      </c>
-      <c r="I7">
-        <v>128.79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>409</v>
-      </c>
-      <c r="E8">
-        <v>40</v>
-      </c>
-      <c r="F8">
-        <v>75</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>225</v>
-      </c>
-      <c r="I8">
-        <v>3225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>403</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>950</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <v>356.25</v>
-      </c>
-      <c r="I9">
-        <v>5106.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>407</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>24.99</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>18.739999999999998</v>
-      </c>
-      <c r="I10">
-        <v>268.64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J9"/>
@@ -4474,8 +4474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="H26" sqref="A26:XFD1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6404,7 +6404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -6917,17 +6917,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="A18:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>

</xml_diff>